<commit_message>
Simu montage Ball Launcher protection...
</commit_message>
<xml_diff>
--- a/_Hard/2014_BallLauncher/Ball_Launcher_Calculs.xlsx
+++ b/_Hard/2014_BallLauncher/Ball_Launcher_Calculs.xlsx
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -199,6 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +497,7 @@
   <dimension ref="D2:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -975,59 +976,59 @@
       <c r="F12" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="10">
         <f>SQRT(H3/PI())*2</f>
         <v>0.252313252202016</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="10">
         <f>SQRT(I3/PI())*2</f>
         <v>0.3989422804014327</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="10">
         <f>SQRT(J3/PI())*2</f>
         <v>0.50462650440403201</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="10">
         <f>SQRT(K3/PI())*2</f>
         <v>0.54115163798060095</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="10">
         <f>SQRT(L3/PI())*2</f>
         <v>0.55279063915413673</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="10">
         <f>SQRT(M3/PI())*2</f>
         <v>0.56418958354775628</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="10">
         <f>SQRT(N3/PI())*2</f>
         <v>0.57536273917515923</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="10">
         <f>SQRT(O3/PI())*2</f>
         <v>0.59708213214418471</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="10">
         <f>SQRT(P3/PI())*2</f>
         <v>0.61803872323710329</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12" s="10">
         <f>SQRT(Q3/PI())*2</f>
         <v>0.7136496464611084</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="10">
         <f>SQRT(R3/PI())*2</f>
         <v>0.79788456080286541</v>
       </c>
-      <c r="S12" s="3">
+      <c r="S12" s="10">
         <f>SQRT(S3/PI())*2</f>
         <v>0.87403874447366325</v>
       </c>
-      <c r="T12" s="3">
+      <c r="T12" s="10">
         <f>SQRT(T3/PI())*2</f>
         <v>0.94406974388262965</v>
       </c>
-      <c r="U12" s="3">
+      <c r="U12" s="10">
         <f>SQRT(U3/PI())*2</f>
         <v>1.009253008808064</v>
       </c>

</xml_diff>

<commit_message>
modif calcul ball launcher
</commit_message>
<xml_diff>
--- a/_Hard/2014_BallLauncher/Ball_Launcher_Calculs.xlsx
+++ b/_Hard/2014_BallLauncher/Ball_Launcher_Calculs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="23475" windowHeight="9495"/>
@@ -11,7 +11,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -132,12 +132,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,26 +186,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -284,6 +288,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -318,6 +323,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,14 +499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
@@ -509,37 +515,37 @@
     <col min="8" max="21" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:22">
+    <row r="2" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-    </row>
-    <row r="3" spans="4:22">
-      <c r="D3" s="7" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+    </row>
+    <row r="3" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>0.25</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="5">
@@ -589,14 +595,14 @@
         <v>mm²</v>
       </c>
     </row>
-    <row r="4" spans="4:22">
-      <c r="D4" s="7" t="s">
+    <row r="4" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>40</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H4">
@@ -660,14 +666,14 @@
         <v>mm</v>
       </c>
     </row>
-    <row r="5" spans="4:22">
-      <c r="D5" s="7" t="s">
+    <row r="5" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>38</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H5">
@@ -731,85 +737,85 @@
         <v>mm</v>
       </c>
     </row>
-    <row r="6" spans="4:22">
-      <c r="D6" s="7" t="s">
+    <row r="6" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7">
-        <v>8</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H6">
         <f>$E$6</f>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6:U6" si="3">$E$6</f>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="J6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="P6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="Q6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="R6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="S6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="T6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" si="1"/>
         <v>mm</v>
       </c>
     </row>
-    <row r="7" spans="4:22">
-      <c r="D7" s="7" t="s">
+    <row r="7" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>24</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H7">
@@ -873,14 +879,14 @@
         <v>V</v>
       </c>
     </row>
-    <row r="8" spans="4:22">
-      <c r="D8" s="7" t="s">
+    <row r="8" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7">
-        <v>5</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="6">
+        <v>5</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H8">
@@ -944,15 +950,15 @@
         <v>A</v>
       </c>
     </row>
-    <row r="9" spans="4:22">
-      <c r="D9" s="7" t="s">
+    <row r="9" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f>1.7*0.00000001</f>
         <v>1.7E-8</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>35</v>
       </c>
       <c r="V9" t="str">
@@ -960,12 +966,12 @@
         <v>ohm*m</v>
       </c>
     </row>
-    <row r="11" spans="4:22">
+    <row r="11" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="4:22">
+    <row r="12" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>8</v>
       </c>
@@ -976,60 +982,60 @@
       <c r="F12" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="10">
-        <f>SQRT(H3/PI())*2</f>
+      <c r="H12" s="3">
+        <f t="shared" ref="H12:U12" si="6">SQRT(H3/PI())*2</f>
         <v>0.252313252202016</v>
       </c>
-      <c r="I12" s="10">
-        <f>SQRT(I3/PI())*2</f>
+      <c r="I12" s="3">
+        <f t="shared" si="6"/>
         <v>0.3989422804014327</v>
       </c>
-      <c r="J12" s="10">
-        <f>SQRT(J3/PI())*2</f>
+      <c r="J12" s="3">
+        <f t="shared" si="6"/>
         <v>0.50462650440403201</v>
       </c>
-      <c r="K12" s="10">
-        <f>SQRT(K3/PI())*2</f>
+      <c r="K12" s="3">
+        <f t="shared" si="6"/>
         <v>0.54115163798060095</v>
       </c>
-      <c r="L12" s="10">
-        <f>SQRT(L3/PI())*2</f>
+      <c r="L12" s="3">
+        <f t="shared" si="6"/>
         <v>0.55279063915413673</v>
       </c>
-      <c r="M12" s="10">
-        <f>SQRT(M3/PI())*2</f>
+      <c r="M12" s="3">
+        <f t="shared" si="6"/>
         <v>0.56418958354775628</v>
       </c>
-      <c r="N12" s="10">
-        <f>SQRT(N3/PI())*2</f>
+      <c r="N12" s="3">
+        <f t="shared" si="6"/>
         <v>0.57536273917515923</v>
       </c>
-      <c r="O12" s="10">
-        <f>SQRT(O3/PI())*2</f>
+      <c r="O12" s="3">
+        <f t="shared" si="6"/>
         <v>0.59708213214418471</v>
       </c>
-      <c r="P12" s="10">
-        <f>SQRT(P3/PI())*2</f>
+      <c r="P12" s="3">
+        <f t="shared" si="6"/>
         <v>0.61803872323710329</v>
       </c>
-      <c r="Q12" s="10">
-        <f>SQRT(Q3/PI())*2</f>
+      <c r="Q12" s="3">
+        <f t="shared" si="6"/>
         <v>0.7136496464611084</v>
       </c>
-      <c r="R12" s="10">
-        <f>SQRT(R3/PI())*2</f>
+      <c r="R12" s="3">
+        <f t="shared" si="6"/>
         <v>0.79788456080286541</v>
       </c>
-      <c r="S12" s="10">
-        <f>SQRT(S3/PI())*2</f>
+      <c r="S12" s="3">
+        <f t="shared" si="6"/>
         <v>0.87403874447366325</v>
       </c>
-      <c r="T12" s="10">
-        <f>SQRT(T3/PI())*2</f>
+      <c r="T12" s="3">
+        <f t="shared" si="6"/>
         <v>0.94406974388262965</v>
       </c>
-      <c r="U12" s="10">
-        <f>SQRT(U3/PI())*2</f>
+      <c r="U12" s="3">
+        <f t="shared" si="6"/>
         <v>1.009253008808064</v>
       </c>
       <c r="V12" t="str">
@@ -1037,151 +1043,151 @@
         <v>mm</v>
       </c>
     </row>
-    <row r="13" spans="4:22">
+    <row r="13" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13">
         <f>(E5-E6)/2</f>
-        <v>15</v>
+        <v>13.75</v>
       </c>
       <c r="F13" t="s">
         <v>1</v>
       </c>
       <c r="H13">
-        <f>(H5-H6)/2</f>
-        <v>15</v>
+        <f t="shared" ref="H13:U13" si="7">(H5-H6)/2</f>
+        <v>13.75</v>
       </c>
       <c r="I13">
-        <f>(I5-I6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="J13">
-        <f>(J5-J6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="K13">
-        <f>(K5-K6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="L13">
-        <f>(L5-L6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="M13">
-        <f>(M5-M6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="N13">
-        <f>(N5-N6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="O13">
-        <f>(O5-O6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="P13">
-        <f>(P5-P6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="Q13">
-        <f>(Q5-Q6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="R13">
-        <f>(R5-R6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="S13">
-        <f>(S5-S6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="T13">
-        <f>(T5-T6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="U13">
-        <f>(U5-U6)/2</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>13.75</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="1"/>
         <v>mm</v>
       </c>
     </row>
-    <row r="14" spans="4:22">
+    <row r="14" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14">
         <f>INT(E13/E12)</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="H14">
-        <f>INT(H13/H12)</f>
-        <v>59</v>
+        <f t="shared" ref="H14:U14" si="8">INT(H13/H12)</f>
+        <v>54</v>
       </c>
       <c r="I14">
-        <f>INT(I13/I12)</f>
-        <v>37</v>
+        <f t="shared" si="8"/>
+        <v>34</v>
       </c>
       <c r="J14">
-        <f>INT(J13/J12)</f>
-        <v>29</v>
+        <f t="shared" si="8"/>
+        <v>27</v>
       </c>
       <c r="K14">
-        <f>INT(K13/K12)</f>
-        <v>27</v>
+        <f t="shared" si="8"/>
+        <v>25</v>
       </c>
       <c r="L14">
-        <f>INT(L13/L12)</f>
-        <v>27</v>
+        <f t="shared" si="8"/>
+        <v>24</v>
       </c>
       <c r="M14">
-        <f>INT(M13/M12)</f>
-        <v>26</v>
+        <f t="shared" si="8"/>
+        <v>24</v>
       </c>
       <c r="N14">
-        <f>INT(N13/N12)</f>
-        <v>26</v>
+        <f t="shared" si="8"/>
+        <v>23</v>
       </c>
       <c r="O14">
-        <f>INT(O13/O12)</f>
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>23</v>
       </c>
       <c r="P14">
-        <f>INT(P13/P12)</f>
-        <v>24</v>
+        <f t="shared" si="8"/>
+        <v>22</v>
       </c>
       <c r="Q14">
-        <f>INT(Q13/Q12)</f>
-        <v>21</v>
+        <f t="shared" si="8"/>
+        <v>19</v>
       </c>
       <c r="R14">
-        <f>INT(R13/R12)</f>
-        <v>18</v>
+        <f t="shared" si="8"/>
+        <v>17</v>
       </c>
       <c r="S14">
-        <f>INT(S13/S12)</f>
-        <v>17</v>
+        <f t="shared" si="8"/>
+        <v>15</v>
       </c>
       <c r="T14">
-        <f>INT(T13/T12)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="U14">
-        <f>INT(U13/U12)</f>
-        <v>14</v>
+        <f t="shared" si="8"/>
+        <v>13</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="1"/>
         <v>fils</v>
       </c>
     </row>
-    <row r="15" spans="4:22">
+    <row r="15" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>11</v>
       </c>
@@ -1193,59 +1199,59 @@
         <v>12</v>
       </c>
       <c r="H15">
-        <f>INT(H4/H12)</f>
+        <f t="shared" ref="H15:U15" si="9">INT(H4/H12)</f>
         <v>158</v>
       </c>
       <c r="I15">
-        <f>INT(I4/I12)</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="J15">
-        <f>INT(J4/J12)</f>
+        <f t="shared" si="9"/>
         <v>79</v>
       </c>
       <c r="K15">
-        <f>INT(K4/K12)</f>
+        <f t="shared" si="9"/>
         <v>73</v>
       </c>
       <c r="L15">
-        <f>INT(L4/L12)</f>
+        <f t="shared" si="9"/>
         <v>72</v>
       </c>
       <c r="M15">
-        <f>INT(M4/M12)</f>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="N15">
-        <f>INT(N4/N12)</f>
+        <f t="shared" si="9"/>
         <v>69</v>
       </c>
       <c r="O15">
-        <f>INT(O4/O12)</f>
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
       <c r="P15">
-        <f>INT(P4/P12)</f>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
       <c r="Q15">
-        <f>INT(Q4/Q12)</f>
+        <f t="shared" si="9"/>
         <v>56</v>
       </c>
       <c r="R15">
-        <f>INT(R4/R12)</f>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="S15">
-        <f>INT(S4/S12)</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="T15">
-        <f>INT(T4/T12)</f>
+        <f t="shared" si="9"/>
         <v>42</v>
       </c>
       <c r="U15">
-        <f>INT(U4/U12)</f>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
       <c r="V15" t="str">
@@ -1253,79 +1259,79 @@
         <v>fils</v>
       </c>
     </row>
-    <row r="16" spans="4:22">
+    <row r="16" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="E16">
         <f>E15*E14</f>
-        <v>1820</v>
+        <v>1680</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
       </c>
       <c r="H16">
-        <f>H15*H14</f>
-        <v>9322</v>
+        <f t="shared" ref="H16:U16" si="10">H15*H14</f>
+        <v>8532</v>
       </c>
       <c r="I16">
-        <f>I15*I14</f>
-        <v>3700</v>
+        <f t="shared" si="10"/>
+        <v>3400</v>
       </c>
       <c r="J16">
-        <f>J15*J14</f>
-        <v>2291</v>
+        <f t="shared" si="10"/>
+        <v>2133</v>
       </c>
       <c r="K16">
-        <f>K15*K14</f>
-        <v>1971</v>
+        <f t="shared" si="10"/>
+        <v>1825</v>
       </c>
       <c r="L16">
-        <f>L15*L14</f>
-        <v>1944</v>
+        <f t="shared" si="10"/>
+        <v>1728</v>
       </c>
       <c r="M16">
-        <f>M15*M14</f>
-        <v>1820</v>
+        <f t="shared" si="10"/>
+        <v>1680</v>
       </c>
       <c r="N16">
-        <f>N15*N14</f>
-        <v>1794</v>
+        <f t="shared" si="10"/>
+        <v>1587</v>
       </c>
       <c r="O16">
-        <f>O15*O14</f>
-        <v>1650</v>
+        <f t="shared" si="10"/>
+        <v>1518</v>
       </c>
       <c r="P16">
-        <f>P15*P14</f>
-        <v>1536</v>
+        <f t="shared" si="10"/>
+        <v>1408</v>
       </c>
       <c r="Q16">
-        <f>Q15*Q14</f>
-        <v>1176</v>
+        <f t="shared" si="10"/>
+        <v>1064</v>
       </c>
       <c r="R16">
-        <f>R15*R14</f>
-        <v>900</v>
+        <f t="shared" si="10"/>
+        <v>850</v>
       </c>
       <c r="S16">
-        <f>S15*S14</f>
-        <v>765</v>
+        <f t="shared" si="10"/>
+        <v>675</v>
       </c>
       <c r="T16">
-        <f>T15*T14</f>
-        <v>630</v>
+        <f t="shared" si="10"/>
+        <v>588</v>
       </c>
       <c r="U16">
-        <f>U15*U14</f>
-        <v>546</v>
+        <f t="shared" si="10"/>
+        <v>507</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="1"/>
         <v>spires</v>
       </c>
     </row>
-    <row r="17" spans="4:22">
+    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>18</v>
       </c>
@@ -1337,59 +1343,59 @@
         <v>15</v>
       </c>
       <c r="H17" s="3">
-        <f>1/(57*H3)</f>
+        <f t="shared" ref="H17:U17" si="11">1/(57*H3)</f>
         <v>0.35087719298245612</v>
       </c>
       <c r="I17" s="3">
-        <f>1/(57*I3)</f>
+        <f t="shared" si="11"/>
         <v>0.14035087719298245</v>
       </c>
       <c r="J17" s="3">
-        <f>1/(57*J3)</f>
+        <f t="shared" si="11"/>
         <v>8.771929824561403E-2</v>
       </c>
       <c r="K17" s="3">
-        <f>1/(57*K3)</f>
+        <f t="shared" si="11"/>
         <v>7.6277650648360021E-2</v>
       </c>
       <c r="L17" s="3">
-        <f>1/(57*L3)</f>
+        <f t="shared" si="11"/>
         <v>7.3099415204678359E-2</v>
       </c>
       <c r="M17" s="3">
-        <f>1/(57*M3)</f>
+        <f t="shared" si="11"/>
         <v>7.0175438596491224E-2</v>
       </c>
       <c r="N17" s="3">
-        <f>1/(57*N3)</f>
+        <f t="shared" si="11"/>
         <v>6.7476383265856948E-2</v>
       </c>
       <c r="O17" s="3">
-        <f>1/(57*O3)</f>
+        <f t="shared" si="11"/>
         <v>6.2656641604010022E-2</v>
       </c>
       <c r="P17" s="3">
-        <f>1/(57*P3)</f>
+        <f t="shared" si="11"/>
         <v>5.8479532163742701E-2</v>
       </c>
       <c r="Q17" s="3">
-        <f>1/(57*Q3)</f>
+        <f t="shared" si="11"/>
         <v>4.3859649122807015E-2</v>
       </c>
       <c r="R17" s="3">
-        <f>1/(57*R3)</f>
+        <f t="shared" si="11"/>
         <v>3.5087719298245612E-2</v>
       </c>
       <c r="S17" s="3">
-        <f>1/(57*S3)</f>
+        <f t="shared" si="11"/>
         <v>2.923976608187135E-2</v>
       </c>
       <c r="T17" s="3">
-        <f>1/(57*T3)</f>
+        <f t="shared" si="11"/>
         <v>2.5062656641604012E-2</v>
       </c>
       <c r="U17" s="3">
-        <f>1/(57*U3)</f>
+        <f t="shared" si="11"/>
         <v>2.1929824561403508E-2</v>
       </c>
       <c r="V17" t="str">
@@ -1397,368 +1403,368 @@
         <v>Ohm/m</v>
       </c>
     </row>
-    <row r="18" spans="4:22">
+    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="3">
         <f>(E14*PI()*E6+E14*(E14+1)/2*E12)*E15/1000</f>
-        <v>59.603727104035762</v>
+        <v>67.26567566382684</v>
       </c>
       <c r="F18" t="s">
         <v>17</v>
       </c>
       <c r="H18" s="3">
-        <f>(H14*PI()*H6+H14*(H14+1)/2*H12)*H15/1000</f>
-        <v>304.84933784492819</v>
+        <f t="shared" ref="H18:U18" si="12">(H14*PI()*H6+H14*(H14+1)/2*H12)*H15/1000</f>
+        <v>340.64297782865424</v>
       </c>
       <c r="I18" s="3">
-        <f>(I14*PI()*I6+I14*(I14+1)/2*I12)*I15/1000</f>
-        <v>121.03678485847858</v>
+        <f t="shared" si="12"/>
+        <v>135.89192341704089</v>
       </c>
       <c r="J18" s="3">
-        <f>(J14*PI()*J6+J14*(J14+1)/2*J12)*J15/1000</f>
-        <v>74.920599978838297</v>
+        <f t="shared" si="12"/>
+        <v>85.429836540636998</v>
       </c>
       <c r="K18" s="3">
-        <f>(K14*PI()*K6+K14*(K14+1)/2*K12)*K15/1000</f>
-        <v>64.469171260240557</v>
+        <f t="shared" si="12"/>
+        <v>73.039591835504169</v>
       </c>
       <c r="L18" s="3">
-        <f>(L14*PI()*L6+L14*(L14+1)/2*L12)*L15/1000</f>
-        <v>63.902798983847447</v>
+        <f t="shared" si="12"/>
+        <v>68.941334912462565</v>
       </c>
       <c r="M18" s="3">
-        <f>(M14*PI()*M6+M14*(M14+1)/2*M12)*M15/1000</f>
-        <v>59.603727104035762</v>
+        <f t="shared" si="12"/>
+        <v>67.26567566382684</v>
       </c>
       <c r="N18" s="3">
-        <f>(N14*PI()*N6+N14*(N14+1)/2*N12)*N15/1000</f>
-        <v>59.0228479444039</v>
+        <f t="shared" si="12"/>
+        <v>63.307137187945258</v>
       </c>
       <c r="O18" s="3">
-        <f>(O14*PI()*O6+O14*(O14+1)/2*O12)*O15/1000</f>
-        <v>54.276434761878029</v>
+        <f t="shared" si="12"/>
+        <v>60.950293424706182</v>
       </c>
       <c r="P18" s="3">
-        <f>(P14*PI()*P6+P14*(P14+1)/2*P12)*P15/1000</f>
-        <v>50.470234013463767</v>
+        <f t="shared" si="12"/>
+        <v>56.452588797326669</v>
       </c>
       <c r="Q18" s="3">
-        <f>(Q14*PI()*Q6+Q14*(Q14+1)/2*Q12)*Q15/1000</f>
-        <v>38.787875511593676</v>
+        <f t="shared" si="12"/>
+        <v>42.691105364251364</v>
       </c>
       <c r="R18" s="3">
-        <f>(R14*PI()*R6+R14*(R14+1)/2*R12)*R15/1000</f>
-        <v>29.441380100711012</v>
+        <f t="shared" si="12"/>
+        <v>34.142531323430823</v>
       </c>
       <c r="S18" s="3">
-        <f>(S14*PI()*S6+S14*(S14+1)/2*S12)*S15/1000</f>
-        <v>25.244303795670707</v>
+        <f t="shared" si="12"/>
+        <v>26.985847152475444</v>
       </c>
       <c r="T18" s="3">
-        <f>(T14*PI()*T6+T14*(T14+1)/2*T12)*T15/1000</f>
-        <v>20.591738483261008</v>
+        <f t="shared" si="12"/>
+        <v>23.559540613785781</v>
       </c>
       <c r="U18" s="3">
-        <f>(U14*PI()*U6+U14*(U14+1)/2*U12)*U15/1000</f>
-        <v>17.855367781949241</v>
+        <f t="shared" si="12"/>
+        <v>20.306107419645084</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="1"/>
         <v>m</v>
       </c>
     </row>
-    <row r="19" spans="4:22">
+    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="3">
         <f>E18*E17</f>
-        <v>4.0530534430744325</v>
+        <v>4.5740659451402257</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="3">
-        <f>H18*H17</f>
-        <v>106.96467994558883</v>
+        <f t="shared" ref="H19:U19" si="13">H18*H17</f>
+        <v>119.52385186970324</v>
       </c>
       <c r="I19" s="3">
-        <f>I18*I17</f>
-        <v>16.987618927505764</v>
+        <f t="shared" si="13"/>
+        <v>19.072550655023282</v>
       </c>
       <c r="J19" s="3">
-        <f>J18*J17</f>
-        <v>6.5719824542840604</v>
+        <f t="shared" si="13"/>
+        <v>7.4938453105821923</v>
       </c>
       <c r="K19" s="3">
-        <f>K18*K17</f>
-        <v>4.917556922977921</v>
+        <f t="shared" si="13"/>
+        <v>5.5712884695273956</v>
       </c>
       <c r="L19" s="3">
-        <f>L18*L17</f>
-        <v>4.6712572356613631</v>
+        <f t="shared" si="13"/>
+        <v>5.0395712655308893</v>
       </c>
       <c r="M19" s="3">
-        <f>M18*M17</f>
-        <v>4.1827176915112814</v>
+        <f t="shared" si="13"/>
+        <v>4.7203982921983743</v>
       </c>
       <c r="N19" s="3">
-        <f>N18*N17</f>
-        <v>3.9826483093389946</v>
+        <f t="shared" si="13"/>
+        <v>4.2717366523579798</v>
       </c>
       <c r="O19" s="3">
-        <f>O18*O17</f>
-        <v>3.4007791204184228</v>
+        <f t="shared" si="13"/>
+        <v>3.8189406907710639</v>
       </c>
       <c r="P19" s="3">
-        <f>P18*P17</f>
-        <v>2.9514756733019754</v>
+        <f t="shared" si="13"/>
+        <v>3.301320982299806</v>
       </c>
       <c r="Q19" s="3">
-        <f>Q18*Q17</f>
-        <v>1.7012226101576173</v>
+        <f t="shared" si="13"/>
+        <v>1.8724169019408492</v>
       </c>
       <c r="R19" s="3">
-        <f>R18*R17</f>
-        <v>1.0330308807267021</v>
+        <f t="shared" si="13"/>
+        <v>1.1979835552080991</v>
       </c>
       <c r="S19" s="3">
-        <f>S18*S17</f>
-        <v>0.7381375378851085</v>
+        <f t="shared" si="13"/>
+        <v>0.78905985825951608</v>
       </c>
       <c r="T19" s="3">
-        <f>T18*T17</f>
-        <v>0.51608367125967447</v>
+        <f t="shared" si="13"/>
+        <v>0.59046467703723771</v>
       </c>
       <c r="U19" s="3">
-        <f>U18*U17</f>
-        <v>0.39156508293748332</v>
+        <f t="shared" si="13"/>
+        <v>0.44530937323783076</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="1"/>
         <v>Ohm</v>
       </c>
     </row>
-    <row r="20" spans="4:22">
+    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="3">
         <f>E7/E19</f>
-        <v>5.9214615195882701</v>
+        <v>5.2469728875463861</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
       </c>
       <c r="H20" s="3">
-        <f>H7/H19</f>
-        <v>0.22437312963688955</v>
+        <f t="shared" ref="H20:U20" si="14">H7/H19</f>
+        <v>0.20079674160905694</v>
       </c>
       <c r="I20" s="3">
-        <f>I7/I19</f>
-        <v>1.4127936412053623</v>
+        <f t="shared" si="14"/>
+        <v>1.2583529300355503</v>
       </c>
       <c r="J20" s="3">
-        <f>J7/J19</f>
-        <v>3.6518661099521323</v>
+        <f t="shared" si="14"/>
+        <v>3.2026281575507269</v>
       </c>
       <c r="K20" s="3">
-        <f>K7/K19</f>
-        <v>4.8804722295855685</v>
+        <f t="shared" si="14"/>
+        <v>4.3078006337797632</v>
       </c>
       <c r="L20" s="3">
-        <f>L7/L19</f>
-        <v>5.1378031200634675</v>
+        <f t="shared" si="14"/>
+        <v>4.7623098742848597</v>
       </c>
       <c r="M20" s="3">
-        <f>M7/M19</f>
-        <v>5.7378962124810355</v>
+        <f t="shared" si="14"/>
+        <v>5.0843167280324497</v>
       </c>
       <c r="N20" s="3">
-        <f>N7/N19</f>
-        <v>6.0261409333387288</v>
+        <f t="shared" si="14"/>
+        <v>5.6183238699305367</v>
       </c>
       <c r="O20" s="3">
-        <f>O7/O19</f>
-        <v>7.0572063489519143</v>
+        <f t="shared" si="14"/>
+        <v>6.2844652335132958</v>
       </c>
       <c r="P20" s="3">
-        <f>P7/P19</f>
-        <v>8.1315256016153779</v>
+        <f t="shared" si="14"/>
+        <v>7.2698171818727033</v>
       </c>
       <c r="Q20" s="3">
-        <f>Q7/Q19</f>
-        <v>14.107501191614432</v>
+        <f t="shared" si="14"/>
+        <v>12.817658276382177</v>
       </c>
       <c r="R20" s="3">
-        <f>R7/R19</f>
-        <v>23.232606544265952</v>
+        <f t="shared" si="14"/>
+        <v>20.033663981164594</v>
       </c>
       <c r="S20" s="3">
-        <f>S7/S19</f>
-        <v>32.514265659438138</v>
+        <f t="shared" si="14"/>
+        <v>30.415943415165561</v>
       </c>
       <c r="T20" s="3">
-        <f>T7/T19</f>
-        <v>46.504087101651535</v>
+        <f t="shared" si="14"/>
+        <v>40.645953828134644</v>
       </c>
       <c r="U20" s="3">
-        <f>U7/U19</f>
-        <v>61.292492731870588</v>
+        <f t="shared" si="14"/>
+        <v>53.895115266711628</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="1"/>
         <v>A</v>
       </c>
     </row>
-    <row r="21" spans="4:22">
+    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="4">
         <f>E20*E7</f>
-        <v>142.11507647011848</v>
+        <v>125.92734930111327</v>
       </c>
       <c r="F21" t="s">
         <v>26</v>
       </c>
       <c r="H21" s="4">
         <f>H20*H7</f>
-        <v>5.3849551112853487</v>
+        <v>4.8191217986173669</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" ref="I21:U21" si="6">I20*I7</f>
-        <v>33.907047388928696</v>
+        <f t="shared" ref="I21:U21" si="15">I20*I7</f>
+        <v>30.200470320853206</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="6"/>
-        <v>87.644786638851173</v>
+        <f t="shared" si="15"/>
+        <v>76.863075781217447</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="6"/>
-        <v>117.13133351005365</v>
+        <f t="shared" si="15"/>
+        <v>103.38721521071432</v>
       </c>
       <c r="L21" s="4">
-        <f t="shared" si="6"/>
-        <v>123.30727488152323</v>
+        <f t="shared" si="15"/>
+        <v>114.29543698283663</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="6"/>
-        <v>137.70950909954485</v>
+        <f t="shared" si="15"/>
+        <v>122.02360147277879</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="6"/>
-        <v>144.62738240012948</v>
+        <f t="shared" si="15"/>
+        <v>134.83977287833289</v>
       </c>
       <c r="O21" s="4">
-        <f t="shared" si="6"/>
-        <v>169.37295237484594</v>
+        <f t="shared" si="15"/>
+        <v>150.82716560431911</v>
       </c>
       <c r="P21" s="4">
-        <f t="shared" si="6"/>
-        <v>195.15661443876905</v>
+        <f t="shared" si="15"/>
+        <v>174.47561236494488</v>
       </c>
       <c r="Q21" s="4">
-        <f t="shared" si="6"/>
-        <v>338.58002859874637</v>
+        <f t="shared" si="15"/>
+        <v>307.62379863317227</v>
       </c>
       <c r="R21" s="4">
-        <f t="shared" si="6"/>
-        <v>557.58255706238288</v>
+        <f t="shared" si="15"/>
+        <v>480.80793554795025</v>
       </c>
       <c r="S21" s="4">
-        <f t="shared" si="6"/>
-        <v>780.34237582651531</v>
+        <f t="shared" si="15"/>
+        <v>729.98264196397349</v>
       </c>
       <c r="T21" s="4">
-        <f t="shared" si="6"/>
-        <v>1116.098090439637</v>
+        <f t="shared" si="15"/>
+        <v>975.5028918752314</v>
       </c>
       <c r="U21" s="4">
-        <f t="shared" si="6"/>
-        <v>1471.0198255648941</v>
+        <f t="shared" si="15"/>
+        <v>1293.4827664010791</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="1"/>
         <v>W</v>
       </c>
     </row>
-    <row r="22" spans="4:22">
-      <c r="D22" s="8" t="s">
+    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <f>4*PI()*0.0000001*E16*E20/(E4/1000)</f>
-        <v>0.3385713241538475</v>
-      </c>
-      <c r="F22" s="8" t="s">
+        <v>0.27692870481528925</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9">
-        <f>4*PI()*0.0000001*H16*H20/(H4/1000)</f>
-        <v>6.5709750317569482E-2</v>
-      </c>
-      <c r="I22" s="9">
-        <f>4*PI()*0.0000001*I16*I20/(I4/1000)</f>
-        <v>0.16422161859721821</v>
-      </c>
-      <c r="J22" s="9">
-        <f>4*PI()*0.0000001*J16*J20/(J4/1000)</f>
-        <v>0.26283900127027782</v>
-      </c>
-      <c r="K22" s="9">
-        <f>4*PI()*0.0000001*K16*K20/(K4/1000)</f>
-        <v>0.30220270189657106</v>
-      </c>
-      <c r="L22" s="9">
-        <f>4*PI()*0.0000001*L16*L20/(L4/1000)</f>
-        <v>0.31377879541059622</v>
-      </c>
-      <c r="M22" s="9">
-        <f>4*PI()*0.0000001*M16*M20/(M4/1000)</f>
-        <v>0.32807561310507838</v>
-      </c>
-      <c r="N22" s="9">
-        <f>4*PI()*0.0000001*N16*N20/(N4/1000)</f>
-        <v>0.33963434073698595</v>
-      </c>
-      <c r="O22" s="9">
-        <f>4*PI()*0.0000001*O16*O20/(O4/1000)</f>
-        <v>0.36581931574212057</v>
-      </c>
-      <c r="P22" s="9">
-        <f>4*PI()*0.0000001*P16*P20/(P4/1000)</f>
-        <v>0.39238565518098728</v>
-      </c>
-      <c r="Q22" s="9">
-        <f>4*PI()*0.0000001*Q16*Q20/(Q4/1000)</f>
-        <v>0.52120345994404138</v>
-      </c>
-      <c r="R22" s="9">
-        <f>4*PI()*0.0000001*R16*R20/(R4/1000)</f>
-        <v>0.6568864743888726</v>
-      </c>
-      <c r="S22" s="9">
-        <f>4*PI()*0.0000001*S16*S20/(S4/1000)</f>
-        <v>0.78142132271406672</v>
-      </c>
-      <c r="T22" s="9">
-        <f>4*PI()*0.0000001*T16*T20/(T4/1000)</f>
-        <v>0.92041045992282444</v>
-      </c>
-      <c r="U22" s="9">
-        <f>4*PI()*0.0000001*U16*U20/(U4/1000)</f>
-        <v>1.0513560050811113</v>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8">
+        <f t="shared" ref="H22:U22" si="16">4*PI()*0.0000001*H16*H20/(H4/1000)</f>
+        <v>5.382169620767862E-2</v>
+      </c>
+      <c r="I22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.13440989890117777</v>
+      </c>
+      <c r="J22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.21460866145110533</v>
+      </c>
+      <c r="K22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.24698372554186826</v>
+      </c>
+      <c r="L22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.25853018771816261</v>
+      </c>
+      <c r="M22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.2683439149660154</v>
+      </c>
+      <c r="N22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.28011319687480718</v>
+      </c>
+      <c r="O22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.29970222850586975</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.3215703638612909</v>
+      </c>
+      <c r="Q22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.42845004186254287</v>
+      </c>
+      <c r="R22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.53496969849556175</v>
+      </c>
+      <c r="S22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.644992904599337</v>
+      </c>
+      <c r="T22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.75083501607435221</v>
+      </c>
+      <c r="U22" s="8">
+        <f t="shared" si="16"/>
+        <v>0.85843464580442119</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="23" spans="4:22">
+    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1774,7 +1780,7 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="4:22">
+    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1790,7 +1796,7 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" spans="4:22">
+    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1806,7 +1812,7 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
     </row>
-    <row r="26" spans="4:22">
+    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>29</v>
       </c>
@@ -1818,59 +1824,59 @@
         <v>24</v>
       </c>
       <c r="H26" s="3">
-        <f>MIN(5,H20)</f>
-        <v>0.22437312963688955</v>
+        <f t="shared" ref="H26:U26" si="17">MIN(5,H20)</f>
+        <v>0.20079674160905694</v>
       </c>
       <c r="I26" s="3">
-        <f>MIN(5,I20)</f>
-        <v>1.4127936412053623</v>
+        <f t="shared" si="17"/>
+        <v>1.2583529300355503</v>
       </c>
       <c r="J26" s="3">
-        <f>MIN(5,J20)</f>
-        <v>3.6518661099521323</v>
+        <f t="shared" si="17"/>
+        <v>3.2026281575507269</v>
       </c>
       <c r="K26" s="3">
-        <f>MIN(5,K20)</f>
-        <v>4.8804722295855685</v>
+        <f t="shared" si="17"/>
+        <v>4.3078006337797632</v>
       </c>
       <c r="L26" s="3">
-        <f>MIN(5,L20)</f>
-        <v>5</v>
+        <f t="shared" si="17"/>
+        <v>4.7623098742848597</v>
       </c>
       <c r="M26" s="3">
-        <f>MIN(5,M20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="N26" s="3">
-        <f>MIN(5,N20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="O26" s="3">
-        <f>MIN(5,O20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P26" s="3">
-        <f>MIN(5,P20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="Q26" s="3">
-        <f>MIN(5,Q20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="R26" s="3">
-        <f>MIN(5,R20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="S26" s="3">
-        <f>MIN(5,S20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="T26" s="3">
-        <f>MIN(5,T20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="U26" s="3">
-        <f>MIN(5,U20)</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="V26" t="str">
@@ -1878,13 +1884,13 @@
         <v>A</v>
       </c>
     </row>
-    <row r="27" spans="4:22">
+    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="3">
         <f>MAX(0,E7/E8 - E19)</f>
-        <v>0.74694655692556733</v>
+        <v>0.22593405485977414</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
@@ -1894,63 +1900,63 @@
         <v>0</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" ref="I27:U27" si="7">MAX(0,I7/I8 - I19)</f>
+        <f t="shared" ref="I27:U27" si="18">MAX(0,I7/I8 - I19)</f>
         <v>0</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L27" s="3">
-        <f t="shared" si="7"/>
-        <v>0.12874276433863674</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="M27" s="3">
-        <f t="shared" si="7"/>
-        <v>0.61728230848871846</v>
+        <f t="shared" si="18"/>
+        <v>7.9601707801625565E-2</v>
       </c>
       <c r="N27" s="3">
-        <f t="shared" si="7"/>
-        <v>0.81735169066100521</v>
+        <f t="shared" si="18"/>
+        <v>0.52826334764201999</v>
       </c>
       <c r="O27" s="3">
-        <f t="shared" si="7"/>
-        <v>1.399220879581577</v>
+        <f t="shared" si="18"/>
+        <v>0.98105930922893592</v>
       </c>
       <c r="P27" s="3">
-        <f t="shared" si="7"/>
-        <v>1.8485243266980245</v>
+        <f t="shared" si="18"/>
+        <v>1.4986790177001938</v>
       </c>
       <c r="Q27" s="3">
-        <f t="shared" si="7"/>
-        <v>3.0987773898423825</v>
+        <f t="shared" si="18"/>
+        <v>2.9275830980591504</v>
       </c>
       <c r="R27" s="3">
-        <f t="shared" si="7"/>
-        <v>3.7669691192732975</v>
+        <f t="shared" si="18"/>
+        <v>3.602016444791901</v>
       </c>
       <c r="S27" s="3">
-        <f t="shared" si="7"/>
-        <v>4.0618624621148918</v>
+        <f t="shared" si="18"/>
+        <v>4.010940141740484</v>
       </c>
       <c r="T27" s="3">
-        <f t="shared" si="7"/>
-        <v>4.2839163287403252</v>
+        <f t="shared" si="18"/>
+        <v>4.2095353229627621</v>
       </c>
       <c r="U27" s="3">
-        <f t="shared" si="7"/>
-        <v>4.4084349170625163</v>
+        <f t="shared" si="18"/>
+        <v>4.354690626762169</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="1"/>
         <v>Ohm</v>
       </c>
     </row>
-    <row r="28" spans="4:22">
+    <row r="28" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>34</v>
       </c>
@@ -1962,59 +1968,59 @@
         <v>26</v>
       </c>
       <c r="H28" s="4">
-        <f>H26*H7</f>
-        <v>5.3849551112853487</v>
+        <f t="shared" ref="H28:U28" si="19">H26*H7</f>
+        <v>4.8191217986173669</v>
       </c>
       <c r="I28" s="4">
-        <f>I26*I7</f>
-        <v>33.907047388928696</v>
+        <f t="shared" si="19"/>
+        <v>30.200470320853206</v>
       </c>
       <c r="J28" s="4">
-        <f>J26*J7</f>
-        <v>87.644786638851173</v>
+        <f t="shared" si="19"/>
+        <v>76.863075781217447</v>
       </c>
       <c r="K28" s="4">
-        <f>K26*K7</f>
-        <v>117.13133351005365</v>
+        <f t="shared" si="19"/>
+        <v>103.38721521071432</v>
       </c>
       <c r="L28" s="4">
-        <f>L26*L7</f>
+        <f t="shared" si="19"/>
+        <v>114.29543698283663</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="M28" s="4">
-        <f>M26*M7</f>
+      <c r="N28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="N28" s="4">
-        <f>N26*N7</f>
+      <c r="O28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="O28" s="4">
-        <f>O26*O7</f>
+      <c r="P28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="P28" s="4">
-        <f>P26*P7</f>
+      <c r="Q28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="Q28" s="4">
-        <f>Q26*Q7</f>
+      <c r="R28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="R28" s="4">
-        <f>R26*R7</f>
+      <c r="S28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="S28" s="4">
-        <f>S26*S7</f>
+      <c r="T28" s="4">
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="T28" s="4">
-        <f>T26*T7</f>
-        <v>120</v>
-      </c>
       <c r="U28" s="4">
-        <f>U26*U7</f>
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
       <c r="V28" t="str">
@@ -2022,72 +2028,72 @@
         <v>W</v>
       </c>
     </row>
-    <row r="29" spans="4:22">
+    <row r="29" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>27</v>
       </c>
       <c r="E29">
         <f>4*PI()*0.0000001*E16*E26/(E4/1000)</f>
-        <v>0.28588493147667116</v>
+        <v>0.26389378290154264</v>
       </c>
       <c r="F29" t="s">
         <v>28</v>
       </c>
       <c r="H29" s="2">
-        <f>4*PI()*0.0000001*H16*H26/(H4/1000)</f>
-        <v>6.5709750317569482E-2</v>
+        <f t="shared" ref="H29:U29" si="20">4*PI()*0.0000001*H16*H26/(H4/1000)</f>
+        <v>5.382169620767862E-2</v>
       </c>
       <c r="I29" s="2">
-        <f>4*PI()*0.0000001*I16*I26/(I4/1000)</f>
-        <v>0.16422161859721821</v>
+        <f t="shared" si="20"/>
+        <v>0.13440989890117777</v>
       </c>
       <c r="J29" s="2">
-        <f>4*PI()*0.0000001*J16*J26/(J4/1000)</f>
-        <v>0.26283900127027782</v>
+        <f t="shared" si="20"/>
+        <v>0.21460866145110533</v>
       </c>
       <c r="K29" s="2">
-        <f>4*PI()*0.0000001*K16*K26/(K4/1000)</f>
-        <v>0.30220270189657106</v>
+        <f t="shared" si="20"/>
+        <v>0.24698372554186826</v>
       </c>
       <c r="L29" s="2">
-        <f>4*PI()*0.0000001*L16*L26/(L4/1000)</f>
-        <v>0.30536280592892795</v>
+        <f t="shared" si="20"/>
+        <v>0.25853018771816261</v>
       </c>
       <c r="M29" s="2">
-        <f>4*PI()*0.0000001*M16*M26/(M4/1000)</f>
-        <v>0.28588493147667116</v>
+        <f t="shared" si="20"/>
+        <v>0.26389378290154264</v>
       </c>
       <c r="N29" s="2">
-        <f>4*PI()*0.0000001*N16*N26/(N4/1000)</f>
-        <v>0.28180086102700441</v>
+        <f t="shared" si="20"/>
+        <v>0.24928537706235013</v>
       </c>
       <c r="O29" s="2">
-        <f>4*PI()*0.0000001*O16*O26/(O4/1000)</f>
-        <v>0.25918139392115791</v>
+        <f t="shared" si="20"/>
+        <v>0.23844688240746528</v>
       </c>
       <c r="P29" s="2">
-        <f>4*PI()*0.0000001*P16*P26/(P4/1000)</f>
-        <v>0.24127431579569611</v>
+        <f t="shared" si="20"/>
+        <v>0.22116812281272141</v>
       </c>
       <c r="Q29" s="2">
-        <f>4*PI()*0.0000001*Q16*Q26/(Q4/1000)</f>
-        <v>0.18472564803107983</v>
+        <f t="shared" si="20"/>
+        <v>0.16713272917097699</v>
       </c>
       <c r="R29" s="2">
-        <f>4*PI()*0.0000001*R16*R26/(R4/1000)</f>
-        <v>0.14137166941154067</v>
+        <f t="shared" si="20"/>
+        <v>0.13351768777756623</v>
       </c>
       <c r="S29" s="2">
-        <f>4*PI()*0.0000001*S16*S26/(S4/1000)</f>
-        <v>0.12016591899980959</v>
+        <f t="shared" si="20"/>
+        <v>0.10602875205865551</v>
       </c>
       <c r="T29" s="2">
-        <f>4*PI()*0.0000001*T16*T26/(T4/1000)</f>
-        <v>9.8960168588078504E-2</v>
+        <f t="shared" si="20"/>
+        <v>9.2362824015539913E-2</v>
       </c>
       <c r="U29" s="2">
-        <f>4*PI()*0.0000001*U16*U26/(U4/1000)</f>
-        <v>8.576547944300135E-2</v>
+        <f t="shared" si="20"/>
+        <v>7.9639373768501248E-2</v>
       </c>
       <c r="V29" t="str">
         <f t="shared" si="1"/>
@@ -2101,9 +2107,9 @@
   <conditionalFormatting sqref="H29:U29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2116,24 +2122,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>